<commit_message>
update testcase chi tiet
</commit_message>
<xml_diff>
--- a/BAOCAO/Testcase/MOBILESHOP_TestcaseDetail.xlsx
+++ b/BAOCAO/Testcase/MOBILESHOP_TestcaseDetail.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="9" activeTab="11"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="10" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Bìa" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="231">
   <si>
     <t>TESTCASE
 WEBSITE BÁN ĐIỆN THOẠI DI ĐỘNG</t>
@@ -607,12 +607,6 @@
     <t>Chưa kiểm tra sản phẩm đăng nằm trong đơn hàng</t>
   </si>
   <si>
-    <t>1.9</t>
-  </si>
-  <si>
-    <t>1.10</t>
-  </si>
-  <si>
     <t>Xem chi tiết đơn hàng</t>
   </si>
   <si>
@@ -620,6 +614,151 @@
   </si>
   <si>
     <t>Hiển thị chi tiết thông tin của đơn hàng</t>
+  </si>
+  <si>
+    <t>Kiểm tra đơn hàng theo trạng thái</t>
+  </si>
+  <si>
+    <t>Hiển thị các đơn hàng theo trạng thái được chọn</t>
+  </si>
+  <si>
+    <t>Duyệt đơn hàng</t>
+  </si>
+  <si>
+    <t>Kiểm tra duyệt đơn hàng</t>
+  </si>
+  <si>
+    <t>Chọn nhân viên giao hàng</t>
+  </si>
+  <si>
+    <t>Kiểm tra chọn nhân viên giao hàng</t>
+  </si>
+  <si>
+    <t>Hiển thị cửa sổ chọn nhân viên giao hàng
+Cập nhật trạng thái đơn hàng thành đang giao sau khi chọn nhân viên</t>
+  </si>
+  <si>
+    <t>Thông báo duyệt đơn hàng thành công
+Cập nhật trạng thái đơn hàng thành đã duyệt nếu xác nhận duyệt đơn
+Cập nhật trạng thái đơn hàng thành đã hủy nếu hủy đơn</t>
+  </si>
+  <si>
+    <t>Hiển thị thông báo cập nhật trạng thái đơn hàng thành công
+Cập nhật trạng thái đơn hàng thành đã giao</t>
+  </si>
+  <si>
+    <t>Duyệt giao hàng thất bại</t>
+  </si>
+  <si>
+    <t>Duyệt giao hàng thành công</t>
+  </si>
+  <si>
+    <t>Kiểm tra duyệt giao hàng thành công</t>
+  </si>
+  <si>
+    <t>Hiển thị thông báo cập nhật trạng thái đơn hàng thành công
+Cập nhật trạng thái đơn hàng thành đã hủy</t>
+  </si>
+  <si>
+    <t>Thông báo mã đơn đặt hàng không được rỗng</t>
+  </si>
+  <si>
+    <t>Kiểm tra mã đơn đặt hàng rỗng</t>
+  </si>
+  <si>
+    <t>Kiểm tra trùng mã đơn đặt hàng</t>
+  </si>
+  <si>
+    <t>Thông báo mã đơn đặt hàng đã tồn tại</t>
+  </si>
+  <si>
+    <t>Kiểm tra duyệt giao hàng thất bại</t>
+  </si>
+  <si>
+    <t>Kiểm tra tạo đơn đặt hàng thành công</t>
+  </si>
+  <si>
+    <t>Thông báo tạo đơn đặt hàng thành công
+Hiển thị đơn đặt hàng vừa tạo</t>
+  </si>
+  <si>
+    <t>Thêm đặt hàng nhà cung cấp</t>
+  </si>
+  <si>
+    <t>Thêm chi tiết đặt hàng nhà cung cấp</t>
+  </si>
+  <si>
+    <t>Thông báo thêm thành công
+Cập nhật vào đơn đặt hàng</t>
+  </si>
+  <si>
+    <t>Hiển thị doanh thu tất cả đơn hàng trong khoảng thời gian được chọn</t>
+  </si>
+  <si>
+    <t>Thông kê doanh thu đơn hàng theo khoảng thời gian</t>
+  </si>
+  <si>
+    <t>Kiểm tra thống kê doanh thu đơn hàng theo khoản thời gian</t>
+  </si>
+  <si>
+    <t>Ngày bắt đằu: 01/01/2023
+Ngày kết thúc: 31/1/2023</t>
+  </si>
+  <si>
+    <t>Lập phiếu nhập</t>
+  </si>
+  <si>
+    <t>Kiểm tra mã phiếu nhập rỗng</t>
+  </si>
+  <si>
+    <t>Thông báo mã phiếu nhập không được trống</t>
+  </si>
+  <si>
+    <t>Kiểm tra trùng mã phiếu nhập</t>
+  </si>
+  <si>
+    <t>Thông báo mã phiếu nhập đã tồn tại</t>
+  </si>
+  <si>
+    <t>Kiểm tra lập phiếu nhập thành công</t>
+  </si>
+  <si>
+    <t>Thông báo tạo phiếu nhập thành thông
+Hiển thi phiếu nhập vừa tạo</t>
+  </si>
+  <si>
+    <t>Kiểm tra nhập hàng từ phiếu nhập</t>
+  </si>
+  <si>
+    <t>Thông báo nhập hàng thành công
+Cập nhật lại số lượng sản phẩm</t>
+  </si>
+  <si>
+    <t>Mã PN đã có: PN001
+Mã PN vừa thêm: PN001</t>
+  </si>
+  <si>
+    <t>Mã phiếu nhập: ""</t>
+  </si>
+  <si>
+    <t>CTDDH đã lập: mã DDH: DDH001, maloaisp: SSA23
+CTDDH vừa thêm: mã DDH: DDH001, maloaisp: SSA23</t>
+  </si>
+  <si>
+    <t>Kiểm tra trùng chi tiết đặt hàng</t>
+  </si>
+  <si>
+    <t>Thông báo chi tiết đặt hàng đã tồn tại</t>
+  </si>
+  <si>
+    <t>Kiểm tra thêm chi tiết đặt hàng thành công</t>
+  </si>
+  <si>
+    <t>Mã DDH: DDH001
+Mã sản phẩm: SSA23</t>
+  </si>
+  <si>
+    <t>Mã sản phẩm: ""</t>
   </si>
 </sst>
 </file>
@@ -806,7 +945,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -871,6 +1010,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -936,6 +1085,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1255,54 +1410,54 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
     </row>
     <row r="3" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
     </row>
     <row r="4" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
     </row>
     <row r="5" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
     </row>
     <row r="9" spans="4:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D9" s="2"/>
@@ -1374,69 +1529,69 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="38"/>
-      <c r="L5" s="29" t="s">
+      <c r="K5" s="42"/>
+      <c r="L5" s="33" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="30"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
       <c r="J6" s="11" t="s">
         <v>39</v>
       </c>
       <c r="K6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="30"/>
+      <c r="L6" s="34"/>
     </row>
     <row r="7" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
@@ -1491,10 +1646,10 @@
       <c r="L8" s="17"/>
     </row>
     <row r="9" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="39" t="s">
         <v>151</v>
       </c>
       <c r="D9" s="24" t="s">
@@ -1516,8 +1671,8 @@
       <c r="L9" s="17"/>
     </row>
     <row r="10" spans="2:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="B10" s="46"/>
-      <c r="C10" s="47"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="51"/>
       <c r="D10" s="24" t="s">
         <v>154</v>
       </c>
@@ -1539,8 +1694,8 @@
       <c r="L10" s="17"/>
     </row>
     <row r="11" spans="2:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="B11" s="34"/>
-      <c r="C11" s="36"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="40"/>
       <c r="D11" s="24" t="s">
         <v>156</v>
       </c>
@@ -1639,8 +1794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L13"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1657,69 +1812,69 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="38"/>
-      <c r="L5" s="29" t="s">
+      <c r="K5" s="42"/>
+      <c r="L5" s="33" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="30"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
       <c r="J6" s="11" t="s">
         <v>39</v>
       </c>
       <c r="K6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="30"/>
+      <c r="L6" s="34"/>
     </row>
     <row r="7" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
@@ -1774,10 +1929,10 @@
       <c r="L8" s="17"/>
     </row>
     <row r="9" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="47" t="s">
         <v>168</v>
       </c>
       <c r="D9" s="24" t="s">
@@ -1786,7 +1941,9 @@
       <c r="E9" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="17"/>
+      <c r="F9" s="17" t="s">
+        <v>230</v>
+      </c>
       <c r="G9" s="17"/>
       <c r="H9" s="24" t="s">
         <v>170</v>
@@ -1801,8 +1958,8 @@
       <c r="L9" s="17"/>
     </row>
     <row r="10" spans="2:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="B10" s="46"/>
-      <c r="C10" s="44"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="48"/>
       <c r="D10" s="24" t="s">
         <v>171</v>
       </c>
@@ -1826,8 +1983,8 @@
       <c r="L10" s="17"/>
     </row>
     <row r="11" spans="2:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="B11" s="34"/>
-      <c r="C11" s="45"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="49"/>
       <c r="D11" s="24" t="s">
         <v>173</v>
       </c>
@@ -1875,7 +2032,7 @@
       </c>
       <c r="L12" s="17"/>
     </row>
-    <row r="13" spans="2:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" ht="75" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
         <v>54</v>
       </c>
@@ -1926,10 +2083,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L16"/>
+  <dimension ref="B2:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1945,69 +2102,69 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="38"/>
-      <c r="L5" s="29" t="s">
+      <c r="K5" s="42"/>
+      <c r="L5" s="33" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="30"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
       <c r="J6" s="11" t="s">
         <v>39</v>
       </c>
       <c r="K6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="30"/>
+      <c r="L6" s="34"/>
     </row>
     <row r="7" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
@@ -2039,16 +2196,18 @@
         <v>43</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>187</v>
-      </c>
-      <c r="E8" s="17"/>
+        <v>185</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>66</v>
+      </c>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
       <c r="H8" s="24" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I8" s="17" t="s">
         <v>77</v>
@@ -2064,16 +2223,18 @@
         <v>44</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>46</v>
+        <v>142</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="17"/>
+        <v>187</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>66</v>
+      </c>
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
       <c r="H9" s="24" t="s">
-        <v>68</v>
+        <v>188</v>
       </c>
       <c r="I9" s="17" t="s">
         <v>77</v>
@@ -2084,21 +2245,23 @@
       </c>
       <c r="L9" s="17"/>
     </row>
-    <row r="10" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" ht="105" x14ac:dyDescent="0.25">
       <c r="B10" s="25" t="s">
         <v>45</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>46</v>
+        <v>189</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="17"/>
+        <v>190</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>66</v>
+      </c>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
       <c r="H10" s="24" t="s">
-        <v>68</v>
+        <v>194</v>
       </c>
       <c r="I10" s="17" t="s">
         <v>77</v>
@@ -2109,21 +2272,23 @@
       </c>
       <c r="L10" s="17"/>
     </row>
-    <row r="11" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" ht="75" x14ac:dyDescent="0.25">
       <c r="B11" s="25" t="s">
         <v>54</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>46</v>
+        <v>191</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="17"/>
+        <v>192</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>66</v>
+      </c>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
       <c r="H11" s="24" t="s">
-        <v>68</v>
+        <v>193</v>
       </c>
       <c r="I11" s="17" t="s">
         <v>77</v>
@@ -2134,21 +2299,23 @@
       </c>
       <c r="L11" s="17"/>
     </row>
-    <row r="12" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" ht="75" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
         <v>55</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>46</v>
+        <v>197</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" s="17"/>
+        <v>198</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>66</v>
+      </c>
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
       <c r="H12" s="24" t="s">
-        <v>68</v>
+        <v>195</v>
       </c>
       <c r="I12" s="17" t="s">
         <v>77</v>
@@ -2159,21 +2326,23 @@
       </c>
       <c r="L12" s="17"/>
     </row>
-    <row r="13" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" ht="75" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
         <v>56</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>46</v>
+        <v>196</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="17"/>
+        <v>204</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>66</v>
+      </c>
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
       <c r="H13" s="24" t="s">
-        <v>68</v>
+        <v>199</v>
       </c>
       <c r="I13" s="17" t="s">
         <v>77</v>
@@ -2183,81 +2352,6 @@
         <v>78</v>
       </c>
       <c r="L13" s="17"/>
-    </row>
-    <row r="14" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="I14" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="J14" s="17"/>
-      <c r="K14" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="L14" s="17"/>
-    </row>
-    <row r="15" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="I15" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="J15" s="17"/>
-      <c r="K15" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="L15" s="17"/>
-    </row>
-    <row r="16" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="I16" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="J16" s="17"/>
-      <c r="K16" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="L16" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -2279,80 +2373,90 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L7"/>
+  <dimension ref="B2:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:L2"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="38"/>
-      <c r="L5" s="29" t="s">
+      <c r="K5" s="42"/>
+      <c r="L5" s="33" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="30"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
       <c r="J6" s="11" t="s">
         <v>39</v>
       </c>
       <c r="K6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="30"/>
-    </row>
-    <row r="7" spans="2:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="L6" s="34"/>
+    </row>
+    <row r="7" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
         <v>42</v>
       </c>
@@ -2377,8 +2481,137 @@
       </c>
       <c r="L7" s="17"/>
     </row>
+    <row r="8" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>207</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="J8" s="17"/>
+      <c r="K8" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="L8" s="17"/>
+    </row>
+    <row r="9" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="50"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="J9" s="17"/>
+      <c r="K9" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="L9" s="17"/>
+    </row>
+    <row r="10" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B10" s="38"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="J10" s="17"/>
+      <c r="K10" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="L10" s="17"/>
+    </row>
+    <row r="11" spans="2:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="B11" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="52" t="s">
+        <v>208</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>226</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="G11" s="17"/>
+      <c r="H11" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="J11" s="17"/>
+      <c r="K11" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="L11" s="17"/>
+    </row>
+    <row r="12" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B12" s="44"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="53" t="s">
+        <v>229</v>
+      </c>
+      <c r="G12" s="29"/>
+      <c r="H12" s="53" t="s">
+        <v>209</v>
+      </c>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="L12" s="29"/>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="15">
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="B5:B6"/>
@@ -2397,80 +2630,90 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L7"/>
+  <dimension ref="B2:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:L2"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="27.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="38"/>
-      <c r="L5" s="29" t="s">
+      <c r="K5" s="42"/>
+      <c r="L5" s="33" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="30"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
       <c r="J6" s="11" t="s">
         <v>39</v>
       </c>
       <c r="K6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="30"/>
-    </row>
-    <row r="7" spans="2:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="L6" s="34"/>
+    </row>
+    <row r="7" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
         <v>42</v>
       </c>
@@ -2494,6 +2737,35 @@
         <v>78</v>
       </c>
       <c r="L7" s="17"/>
+    </row>
+    <row r="8" spans="2:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="B8" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>211</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="J8" s="17"/>
+      <c r="K8" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="L8" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -2515,80 +2787,90 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L7"/>
+  <dimension ref="B2:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:L2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="38"/>
-      <c r="L5" s="29" t="s">
+      <c r="K5" s="42"/>
+      <c r="L5" s="33" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="30"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
       <c r="J6" s="11" t="s">
         <v>39</v>
       </c>
       <c r="K6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="30"/>
-    </row>
-    <row r="7" spans="2:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="L6" s="34"/>
+    </row>
+    <row r="7" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
         <v>42</v>
       </c>
@@ -2613,8 +2895,110 @@
       </c>
       <c r="L7" s="17"/>
     </row>
+    <row r="8" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="52" t="s">
+        <v>214</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="J8" s="17"/>
+      <c r="K8" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="L8" s="17"/>
+    </row>
+    <row r="9" spans="2:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="B9" s="44"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="26" t="s">
+        <v>217</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>223</v>
+      </c>
+      <c r="G9" s="17"/>
+      <c r="H9" s="26" t="s">
+        <v>218</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="J9" s="17"/>
+      <c r="K9" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="L9" s="17"/>
+    </row>
+    <row r="10" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B10" s="44"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="J10" s="29"/>
+      <c r="K10" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="L10" s="29"/>
+    </row>
+    <row r="11" spans="2:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="B11" s="44"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="J11" s="29"/>
+      <c r="K11" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="L11" s="29"/>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C11"/>
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="B5:B6"/>
@@ -2628,6 +3012,7 @@
     <mergeCell ref="J5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2654,18 +3039,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
     </row>
     <row r="5" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
@@ -2950,69 +3335,69 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="38"/>
-      <c r="L5" s="29" t="s">
+      <c r="K5" s="42"/>
+      <c r="L5" s="33" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
       <c r="J6" s="11" t="s">
         <v>39</v>
       </c>
       <c r="K6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="30"/>
+      <c r="L6" s="34"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
@@ -3192,10 +3577,10 @@
       <c r="L13" s="9"/>
     </row>
     <row r="14" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="39" t="s">
         <v>63</v>
       </c>
       <c r="D14" s="10" t="s">
@@ -3217,8 +3602,8 @@
       <c r="L14" s="9"/>
     </row>
     <row r="15" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B15" s="34"/>
-      <c r="C15" s="36"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="40"/>
       <c r="D15" s="10" t="s">
         <v>65</v>
       </c>
@@ -3281,69 +3666,69 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="38"/>
-      <c r="L5" s="29" t="s">
+      <c r="K5" s="42"/>
+      <c r="L5" s="33" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="30"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
       <c r="J6" s="11" t="s">
         <v>39</v>
       </c>
       <c r="K6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="30"/>
+      <c r="L6" s="34"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
@@ -3371,10 +3756,10 @@
       <c r="L7" s="17"/>
     </row>
     <row r="8" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="43" t="s">
         <v>79</v>
       </c>
       <c r="D8" s="16" t="s">
@@ -3394,8 +3779,8 @@
       <c r="L8" s="17"/>
     </row>
     <row r="9" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="40"/>
-      <c r="C9" s="39"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="43"/>
       <c r="D9" s="16" t="s">
         <v>80</v>
       </c>
@@ -3509,69 +3894,69 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="38"/>
-      <c r="L5" s="29" t="s">
+      <c r="K5" s="42"/>
+      <c r="L5" s="33" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="30"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
       <c r="J6" s="11" t="s">
         <v>39</v>
       </c>
       <c r="K6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="30"/>
+      <c r="L6" s="34"/>
     </row>
     <row r="7" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
@@ -3599,10 +3984,10 @@
       <c r="L7" s="17"/>
     </row>
     <row r="8" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="47" t="s">
         <v>97</v>
       </c>
       <c r="D8" s="19" t="s">
@@ -3624,8 +4009,8 @@
       <c r="L8" s="17"/>
     </row>
     <row r="9" spans="2:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="B9" s="46"/>
-      <c r="C9" s="44"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="48"/>
       <c r="D9" s="19" t="s">
         <v>99</v>
       </c>
@@ -3647,8 +4032,8 @@
       <c r="L9" s="17"/>
     </row>
     <row r="10" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="46"/>
-      <c r="C10" s="44"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="48"/>
       <c r="D10" s="19" t="s">
         <v>100</v>
       </c>
@@ -3670,8 +4055,8 @@
       <c r="L10" s="17"/>
     </row>
     <row r="11" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B11" s="46"/>
-      <c r="C11" s="44"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="48"/>
       <c r="D11" s="19" t="s">
         <v>101</v>
       </c>
@@ -3693,8 +4078,8 @@
       <c r="L11" s="17"/>
     </row>
     <row r="12" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="34"/>
-      <c r="C12" s="45"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="49"/>
       <c r="D12" s="19" t="s">
         <v>102</v>
       </c>
@@ -3783,69 +4168,69 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="38"/>
-      <c r="L5" s="29" t="s">
+      <c r="K5" s="42"/>
+      <c r="L5" s="33" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="30"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
       <c r="J6" s="11" t="s">
         <v>39</v>
       </c>
       <c r="K6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="30"/>
+      <c r="L6" s="34"/>
     </row>
     <row r="7" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
@@ -3965,69 +4350,69 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="38"/>
-      <c r="L5" s="29" t="s">
+      <c r="K5" s="42"/>
+      <c r="L5" s="33" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="30"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
       <c r="J6" s="11" t="s">
         <v>39</v>
       </c>
       <c r="K6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="30"/>
+      <c r="L6" s="34"/>
     </row>
     <row r="7" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
@@ -4174,69 +4559,69 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="38"/>
-      <c r="L5" s="29" t="s">
+      <c r="K5" s="42"/>
+      <c r="L5" s="33" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="30"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
       <c r="J6" s="11" t="s">
         <v>39</v>
       </c>
       <c r="K6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="30"/>
+      <c r="L6" s="34"/>
     </row>
     <row r="7" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
@@ -4383,69 +4768,69 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="38"/>
-      <c r="L5" s="29" t="s">
+      <c r="K5" s="42"/>
+      <c r="L5" s="33" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="30"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
       <c r="J6" s="11" t="s">
         <v>39</v>
       </c>
       <c r="K6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="30"/>
+      <c r="L6" s="34"/>
     </row>
     <row r="7" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">

</xml_diff>